<commit_message>
fix arr creation KR
</commit_message>
<xml_diff>
--- a/Algs/KR_Nikita/Лист Microsoft Excel.xlsx
+++ b/Algs/KR_Nikita/Лист Microsoft Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>Размер</t>
   </si>
@@ -38,7 +38,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -72,7 +72,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1904,18 +1904,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1928,8 +1928,20 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5000</v>
       </c>
@@ -1942,8 +1954,20 @@
       <c r="D2" s="2">
         <v>0.70113999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M2">
+        <v>5000</v>
+      </c>
+      <c r="N2" s="3">
+        <v>14.3593799999999</v>
+      </c>
+      <c r="O2" s="3">
+        <v>4.5294099999999897</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0.70113999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6000</v>
       </c>
@@ -1956,8 +1980,20 @@
       <c r="D3" s="2">
         <v>0.90007999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M3">
+        <v>6000</v>
+      </c>
+      <c r="N3" s="2">
+        <v>12.83365</v>
+      </c>
+      <c r="O3" s="2">
+        <v>3.8898899999999998</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0.90007999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>7000</v>
       </c>
@@ -1970,8 +2006,20 @@
       <c r="D4" s="2">
         <v>0.92313000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M4">
+        <v>7000</v>
+      </c>
+      <c r="N4" s="2">
+        <v>15.991499999999901</v>
+      </c>
+      <c r="O4" s="2">
+        <v>4.4949399999999997</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0.92313000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>8000</v>
       </c>
@@ -1984,8 +2032,20 @@
       <c r="D5" s="2">
         <v>0.58149999999999902</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M5">
+        <v>8000</v>
+      </c>
+      <c r="N5" s="2">
+        <v>24.238399999999999</v>
+      </c>
+      <c r="O5" s="2">
+        <v>6.6419100000000002</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0.58149999999999902</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>9000</v>
       </c>
@@ -1998,8 +2058,20 @@
       <c r="D6" s="2">
         <v>1.0793600000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M6">
+        <v>9000</v>
+      </c>
+      <c r="N6" s="2">
+        <v>28.726099999999999</v>
+      </c>
+      <c r="O6" s="2">
+        <v>8.2780100000000001</v>
+      </c>
+      <c r="P6" s="2">
+        <v>1.0793600000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10000</v>
       </c>
@@ -2012,8 +2084,20 @@
       <c r="D7" s="2">
         <v>0.91942999999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M7">
+        <v>10000</v>
+      </c>
+      <c r="N7" s="2">
+        <v>28.529620000000001</v>
+      </c>
+      <c r="O7" s="2">
+        <v>9.6173599999999997</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0.91942999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>11000</v>
       </c>
@@ -2026,8 +2110,20 @@
       <c r="D8" s="2">
         <v>0.96134999999999904</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M8">
+        <v>11000</v>
+      </c>
+      <c r="N8" s="2">
+        <v>33.809469999999997</v>
+      </c>
+      <c r="O8" s="2">
+        <v>10.824199999999999</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0.96134999999999904</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>12000</v>
       </c>
@@ -2040,8 +2136,20 @@
       <c r="D9" s="2">
         <v>1.2953399999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M9">
+        <v>12000</v>
+      </c>
+      <c r="N9" s="2">
+        <v>40.482709999999997</v>
+      </c>
+      <c r="O9" s="2">
+        <v>10.778</v>
+      </c>
+      <c r="P9" s="2">
+        <v>1.2953399999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>13000</v>
       </c>
@@ -2054,8 +2162,20 @@
       <c r="D10" s="1">
         <v>1.2503899999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M10">
+        <v>13000</v>
+      </c>
+      <c r="N10" s="1">
+        <v>57.411569999999998</v>
+      </c>
+      <c r="O10" s="1">
+        <v>14.24874</v>
+      </c>
+      <c r="P10" s="1">
+        <v>1.2503899999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>14000</v>
       </c>
@@ -2068,8 +2188,20 @@
       <c r="D11" s="1">
         <v>1.4421900000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M11">
+        <v>14000</v>
+      </c>
+      <c r="N11" s="1">
+        <v>52.496339999999996</v>
+      </c>
+      <c r="O11" s="1">
+        <v>16.50028</v>
+      </c>
+      <c r="P11" s="1">
+        <v>1.4421900000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>15000</v>
       </c>
@@ -2082,8 +2214,20 @@
       <c r="D12" s="1">
         <v>1.55514999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M12">
+        <v>15000</v>
+      </c>
+      <c r="N12" s="1">
+        <v>60.916110000000003</v>
+      </c>
+      <c r="O12" s="1">
+        <v>21.920479999999898</v>
+      </c>
+      <c r="P12" s="1">
+        <v>1.55514999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>16000</v>
       </c>
@@ -2096,8 +2240,20 @@
       <c r="D13" s="1">
         <v>4.6166400000000003</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M13">
+        <v>16000</v>
+      </c>
+      <c r="N13" s="1">
+        <v>95.015829999999994</v>
+      </c>
+      <c r="O13" s="1">
+        <v>56.776679999999999</v>
+      </c>
+      <c r="P13" s="1">
+        <v>4.6166400000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>17000</v>
       </c>
@@ -2110,8 +2266,20 @@
       <c r="D14" s="1">
         <v>1.4456800000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M14">
+        <v>17000</v>
+      </c>
+      <c r="N14" s="1">
+        <v>86.277249999999995</v>
+      </c>
+      <c r="O14" s="1">
+        <v>23.40081</v>
+      </c>
+      <c r="P14" s="1">
+        <v>1.4456800000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>18000</v>
       </c>
@@ -2124,8 +2292,20 @@
       <c r="D15" s="1">
         <v>1.4250099999999899</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M15">
+        <v>18000</v>
+      </c>
+      <c r="N15" s="1">
+        <v>98.277150000000006</v>
+      </c>
+      <c r="O15" s="1">
+        <v>26.929559999999999</v>
+      </c>
+      <c r="P15" s="1">
+        <v>1.4250099999999899</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>19000</v>
       </c>
@@ -2138,8 +2318,20 @@
       <c r="D16" s="1">
         <v>1.9488799999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M16">
+        <v>19000</v>
+      </c>
+      <c r="N16" s="1">
+        <v>94.732680000000002</v>
+      </c>
+      <c r="O16" s="1">
+        <v>29.269690000000001</v>
+      </c>
+      <c r="P16" s="1">
+        <v>1.9488799999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>20000</v>
       </c>
@@ -2152,8 +2344,20 @@
       <c r="D17" s="1">
         <v>2.0640100000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M17">
+        <v>20000</v>
+      </c>
+      <c r="N17" s="1">
+        <v>153.60168999999999</v>
+      </c>
+      <c r="O17" s="1">
+        <v>50.087199999999903</v>
+      </c>
+      <c r="P17" s="1">
+        <v>2.0640100000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>21000</v>
       </c>
@@ -2166,8 +2370,20 @@
       <c r="D18" s="1">
         <v>2.3094299999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M18">
+        <v>21000</v>
+      </c>
+      <c r="N18" s="1">
+        <v>169.51212999999899</v>
+      </c>
+      <c r="O18" s="1">
+        <v>56.9017699999999</v>
+      </c>
+      <c r="P18" s="1">
+        <v>2.3094299999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>22000</v>
       </c>
@@ -2180,8 +2396,20 @@
       <c r="D19" s="1">
         <v>3.2714699999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M19">
+        <v>22000</v>
+      </c>
+      <c r="N19" s="1">
+        <v>189.45932999999999</v>
+      </c>
+      <c r="O19" s="1">
+        <v>58.517299999999999</v>
+      </c>
+      <c r="P19" s="1">
+        <v>3.2714699999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>23000</v>
       </c>
@@ -2194,8 +2422,20 @@
       <c r="D20" s="1">
         <v>2.7814099999999899</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M20">
+        <v>23000</v>
+      </c>
+      <c r="N20" s="1">
+        <v>247.07355000000001</v>
+      </c>
+      <c r="O20" s="1">
+        <v>62.552639999999997</v>
+      </c>
+      <c r="P20" s="1">
+        <v>2.7814099999999899</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>24000</v>
       </c>
@@ -2208,8 +2448,20 @@
       <c r="D21" s="1">
         <v>3.4051200000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M21">
+        <v>24000</v>
+      </c>
+      <c r="N21" s="1">
+        <v>236.675669999999</v>
+      </c>
+      <c r="O21" s="1">
+        <v>74.218800000000002</v>
+      </c>
+      <c r="P21" s="1">
+        <v>3.4051200000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>25000</v>
       </c>
@@ -2222,8 +2474,20 @@
       <c r="D22" s="1">
         <v>3.95024</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M22">
+        <v>25000</v>
+      </c>
+      <c r="N22" s="1">
+        <v>236.61043000000001</v>
+      </c>
+      <c r="O22" s="1">
+        <v>81.561599999999999</v>
+      </c>
+      <c r="P22" s="1">
+        <v>3.95024</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>26000</v>
       </c>
@@ -2236,8 +2500,20 @@
       <c r="D23" s="1">
         <v>6.5240099999999996</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M23">
+        <v>26000</v>
+      </c>
+      <c r="N23" s="1">
+        <v>264.737449999999</v>
+      </c>
+      <c r="O23" s="1">
+        <v>131.89983999999899</v>
+      </c>
+      <c r="P23" s="1">
+        <v>6.5240099999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>27000</v>
       </c>
@@ -2250,8 +2526,20 @@
       <c r="D24" s="1">
         <v>3.4136099999999998</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M24">
+        <v>27000</v>
+      </c>
+      <c r="N24" s="1">
+        <v>291.98518000000001</v>
+      </c>
+      <c r="O24" s="1">
+        <v>87.272999999999996</v>
+      </c>
+      <c r="P24" s="1">
+        <v>3.4136099999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>28000</v>
       </c>
@@ -2264,8 +2552,20 @@
       <c r="D25" s="1">
         <v>3.7044700000000002</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M25">
+        <v>28000</v>
+      </c>
+      <c r="N25" s="1">
+        <v>312.06029999999998</v>
+      </c>
+      <c r="O25" s="1">
+        <v>94.243899999999996</v>
+      </c>
+      <c r="P25" s="1">
+        <v>3.7044700000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>29000</v>
       </c>
@@ -2278,8 +2578,20 @@
       <c r="D26" s="1">
         <v>3.4699199999999899</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M26">
+        <v>29000</v>
+      </c>
+      <c r="N26" s="1">
+        <v>340.10120000000001</v>
+      </c>
+      <c r="O26" s="1">
+        <v>101.68519000000001</v>
+      </c>
+      <c r="P26" s="1">
+        <v>3.4699199999999899</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>30000</v>
       </c>
@@ -2292,8 +2604,20 @@
       <c r="D27" s="1">
         <v>2.5130199999999898</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M27">
+        <v>30000</v>
+      </c>
+      <c r="N27" s="1">
+        <v>265.96402999999998</v>
+      </c>
+      <c r="O27" s="1">
+        <v>74.838049999999996</v>
+      </c>
+      <c r="P27" s="1">
+        <v>2.5130199999999898</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>31000</v>
       </c>
@@ -2306,8 +2630,20 @@
       <c r="D28" s="1">
         <v>2.8041799999999899</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M28">
+        <v>31000</v>
+      </c>
+      <c r="N28" s="1">
+        <v>280.26351</v>
+      </c>
+      <c r="O28" s="1">
+        <v>81.476900000000001</v>
+      </c>
+      <c r="P28" s="1">
+        <v>2.8041799999999899</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>32000</v>
       </c>
@@ -2320,8 +2656,20 @@
       <c r="D29" s="1">
         <v>2.5671599999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M29">
+        <v>32000</v>
+      </c>
+      <c r="N29" s="1">
+        <v>331.91807</v>
+      </c>
+      <c r="O29" s="1">
+        <v>85.108260000000001</v>
+      </c>
+      <c r="P29" s="1">
+        <v>2.5671599999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>33000</v>
       </c>
@@ -2334,8 +2682,20 @@
       <c r="D30" s="1">
         <v>2.6003799999999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M30">
+        <v>33000</v>
+      </c>
+      <c r="N30" s="1">
+        <v>300.36007000000001</v>
+      </c>
+      <c r="O30" s="1">
+        <v>90.242339999999899</v>
+      </c>
+      <c r="P30" s="1">
+        <v>2.6003799999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>34000</v>
       </c>
@@ -2348,8 +2708,20 @@
       <c r="D31" s="1">
         <v>3.17821</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="M31">
+        <v>34000</v>
+      </c>
+      <c r="N31" s="1">
+        <v>340.82094999999998</v>
+      </c>
+      <c r="O31" s="1">
+        <v>93.762829999999994</v>
+      </c>
+      <c r="P31" s="1">
+        <v>3.17821</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>35000</v>
       </c>
@@ -2362,8 +2734,20 @@
       <c r="D32" s="1">
         <v>3.5030299999999999</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="M32">
+        <v>35000</v>
+      </c>
+      <c r="N32" s="1">
+        <v>328.24231999999898</v>
+      </c>
+      <c r="O32" s="1">
+        <v>108.34951</v>
+      </c>
+      <c r="P32" s="1">
+        <v>3.5030299999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>

</xml_diff>

<commit_message>
finish exel algs KR
</commit_message>
<xml_diff>
--- a/Algs/KR_Nikita/Лист Microsoft Excel.xlsx
+++ b/Algs/KR_Nikita/Лист Microsoft Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
   <si>
     <t>Размер</t>
   </si>
@@ -106,7 +106,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -274,9 +273,9 @@
             <c:numRef>
               <c:f>Аркуш1!$B$2:$B$32</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
-                <c:pt idx="0" formatCode="General">
+                <c:pt idx="0">
                   <c:v>14.3593799999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -511,9 +510,9 @@
             <c:numRef>
               <c:f>Аркуш1!$C$2:$C$32</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
-                <c:pt idx="0" formatCode="General">
+                <c:pt idx="0">
                   <c:v>4.5294099999999897</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -748,7 +747,7 @@
             <c:numRef>
               <c:f>Аркуш1!$D$2:$D$32</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>0.70113999999999999</c:v>
@@ -983,7 +982,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2968,6 +2966,965 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Аркуш1!$AL$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Выбором</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Аркуш1!$AK$2:$AK$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>28000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>29000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>31000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>34000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>35000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Аркуш1!$AL$2:$AL$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>5.91930599999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7292949999999898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9014869999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.749807000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.319043000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>19.736445</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.970375000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28.864035000000001</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00">
+                  <c:v>33.1413709999999</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00">
+                  <c:v>39.031855999999898</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00">
+                  <c:v>44.075682</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00">
+                  <c:v>50.127304000000002</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.00">
+                  <c:v>56.3362529999999</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.00">
+                  <c:v>63.108265999999901</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.00">
+                  <c:v>70.543727999999902</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.00">
+                  <c:v>77.884429999999995</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.00">
+                  <c:v>85.664824999999993</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="0.00">
+                  <c:v>94.093359999999905</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="0.00">
+                  <c:v>102.523113</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="0.00">
+                  <c:v>111.522629999999</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="0.00">
+                  <c:v>123.110223</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="0.00">
+                  <c:v>131.49254999999999</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="0.00">
+                  <c:v>141.08928699999899</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="0.00">
+                  <c:v>152.36953800000001</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="0.00">
+                  <c:v>163.916898</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="0.00">
+                  <c:v>174.050454</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="0.00">
+                  <c:v>188.60286299999899</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="0.00">
+                  <c:v>200.575853</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="0.00">
+                  <c:v>210.50672599999899</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="0.00">
+                  <c:v>223.73216400000001</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="0.00">
+                  <c:v>237.09723399999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AA31-4EDC-B7A4-D17D7E86E4F7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Аркуш1!$AM$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Вставками</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Аркуш1!$AK$2:$AK$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>28000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>29000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>31000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>34000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>35000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Аркуш1!$AM$2:$AM$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>2.0671309999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3699880000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1073559999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1994389999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1557399999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.382193</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.9512529999999897</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.2328699999999895</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00">
+                  <c:v>10.900321</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00">
+                  <c:v>12.6462489999999</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00">
+                  <c:v>14.379073999999999</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00">
+                  <c:v>16.438334000000001</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.00">
+                  <c:v>18.819907000000001</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.00">
+                  <c:v>20.898319999999899</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.00">
+                  <c:v>23.544235</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.00">
+                  <c:v>25.590960999999901</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.00">
+                  <c:v>28.2793139999999</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="0.00">
+                  <c:v>30.854281999999898</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="0.00">
+                  <c:v>33.615399999999902</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="0.00">
+                  <c:v>36.867277999999999</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="0.00">
+                  <c:v>39.903345000000002</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="0.00">
+                  <c:v>42.991053000000001</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="0.00">
+                  <c:v>46.427185999999999</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="0.00">
+                  <c:v>51.149076999999998</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="0.00">
+                  <c:v>53.728656000000001</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="0.00">
+                  <c:v>59.379022999999897</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="0.00">
+                  <c:v>61.546969999999902</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="0.00">
+                  <c:v>65.790881999999996</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="0.00">
+                  <c:v>70.290911999999906</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="0.00">
+                  <c:v>74.096071999999893</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="0.00">
+                  <c:v>78.308682999999903</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AA31-4EDC-B7A4-D17D7E86E4F7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Аркуш1!$AN$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Слиянием</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Аркуш1!$AK$2:$AK$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>27000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>28000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>29000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>31000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>34000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>35000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Аркуш1!$AN$2:$AN$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0.76664099999999902</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.45596999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.53091500000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.58597200000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.65136299999999903</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.77646399999999904</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0232920000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.97184599999999999</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00">
+                  <c:v>1.0519270000000001</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0.00">
+                  <c:v>1.2426009999999901</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="0.00">
+                  <c:v>1.192161</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00">
+                  <c:v>1.5837459999999901</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="0.00">
+                  <c:v>1.4539679999999999</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="0.00">
+                  <c:v>1.653087</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="0.00">
+                  <c:v>1.553493</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="0.00">
+                  <c:v>1.66315999999999</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.00">
+                  <c:v>1.79426</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="0.00">
+                  <c:v>1.86834199999999</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="0.00">
+                  <c:v>2.0338910000000001</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="0.00">
+                  <c:v>2.0497289999999899</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="0.00">
+                  <c:v>2.6106019999999899</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="0.00">
+                  <c:v>2.7754779999999899</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="0.00">
+                  <c:v>2.385783</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="0.00">
+                  <c:v>2.3556119999999998</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="0.00">
+                  <c:v>2.6308769999999999</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="0.00">
+                  <c:v>2.3992830000000001</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="0.00">
+                  <c:v>2.5101879999999999</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="0.00">
+                  <c:v>5.6361590000000001</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="0.00">
+                  <c:v>3.6168330000000002</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="0.00">
+                  <c:v>4.3688310000000001</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="0.00">
+                  <c:v>3.4384079999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AA31-4EDC-B7A4-D17D7E86E4F7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1038215887"/>
+        <c:axId val="1038227119"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1038215887"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1038227119"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1038227119"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1038215887"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3088,6 +4045,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4121,6 +5118,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4701,15 +6214,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>187325</xdr:colOff>
+      <xdr:colOff>187324</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>492125</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>541019</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>53339</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4723,6 +6236,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Диаграмма 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4994,18 +6537,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB33"/>
+  <dimension ref="A1:AN33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AK10" sqref="AK10"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AV22" sqref="AV22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5042,8 +6585,20 @@
       <c r="AB1" t="s">
         <v>3</v>
       </c>
+      <c r="AK1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5000</v>
       </c>
@@ -5080,8 +6635,20 @@
       <c r="AB2" s="2">
         <v>0.47929299999999903</v>
       </c>
+      <c r="AK2">
+        <v>5000</v>
+      </c>
+      <c r="AL2" s="3">
+        <v>5.91930599999999</v>
+      </c>
+      <c r="AM2" s="3">
+        <v>2.0671309999999998</v>
+      </c>
+      <c r="AN2" s="2">
+        <v>0.76664099999999902</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>6000</v>
       </c>
@@ -5118,8 +6685,20 @@
       <c r="AB3" s="2">
         <v>0.45739099999999999</v>
       </c>
+      <c r="AK3">
+        <v>6000</v>
+      </c>
+      <c r="AL3" s="2">
+        <v>7.7292949999999898</v>
+      </c>
+      <c r="AM3" s="2">
+        <v>2.3699880000000002</v>
+      </c>
+      <c r="AN3" s="2">
+        <v>0.45596999999999999</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>7000</v>
       </c>
@@ -5156,8 +6735,20 @@
       <c r="AB4" s="2">
         <v>0.422376999999999</v>
       </c>
+      <c r="AK4">
+        <v>7000</v>
+      </c>
+      <c r="AL4" s="2">
+        <v>9.9014869999999995</v>
+      </c>
+      <c r="AM4" s="2">
+        <v>3.1073559999999998</v>
+      </c>
+      <c r="AN4" s="2">
+        <v>0.53091500000000003</v>
+      </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>8000</v>
       </c>
@@ -5194,8 +6785,20 @@
       <c r="AB5" s="2">
         <v>0.56025499999999995</v>
       </c>
+      <c r="AK5">
+        <v>8000</v>
+      </c>
+      <c r="AL5" s="2">
+        <v>12.749807000000001</v>
+      </c>
+      <c r="AM5" s="2">
+        <v>4.1994389999999999</v>
+      </c>
+      <c r="AN5" s="2">
+        <v>0.58597200000000005</v>
+      </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>9000</v>
       </c>
@@ -5232,8 +6835,20 @@
       <c r="AB6" s="2">
         <v>0.56605499999999997</v>
       </c>
+      <c r="AK6">
+        <v>9000</v>
+      </c>
+      <c r="AL6" s="2">
+        <v>16.319043000000001</v>
+      </c>
+      <c r="AM6" s="2">
+        <v>5.1557399999999998</v>
+      </c>
+      <c r="AN6" s="2">
+        <v>0.65136299999999903</v>
+      </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10000</v>
       </c>
@@ -5270,8 +6885,20 @@
       <c r="AB7" s="2">
         <v>0.64714099999999897</v>
       </c>
+      <c r="AK7">
+        <v>10000</v>
+      </c>
+      <c r="AL7" s="2">
+        <v>19.736445</v>
+      </c>
+      <c r="AM7" s="2">
+        <v>6.382193</v>
+      </c>
+      <c r="AN7" s="2">
+        <v>0.77646399999999904</v>
+      </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>11000</v>
       </c>
@@ -5308,8 +6935,20 @@
       <c r="AB8" s="2">
         <v>0.72462899999999897</v>
       </c>
+      <c r="AK8">
+        <v>11000</v>
+      </c>
+      <c r="AL8" s="2">
+        <v>23.970375000000001</v>
+      </c>
+      <c r="AM8" s="2">
+        <v>7.9512529999999897</v>
+      </c>
+      <c r="AN8" s="2">
+        <v>1.0232920000000001</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>12000</v>
       </c>
@@ -5346,8 +6985,20 @@
       <c r="AB9" s="2">
         <v>0.86252499999999999</v>
       </c>
+      <c r="AK9">
+        <v>12000</v>
+      </c>
+      <c r="AL9" s="2">
+        <v>28.864035000000001</v>
+      </c>
+      <c r="AM9" s="2">
+        <v>9.2328699999999895</v>
+      </c>
+      <c r="AN9" s="2">
+        <v>0.97184599999999999</v>
+      </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>13000</v>
       </c>
@@ -5384,8 +7035,20 @@
       <c r="AB10" s="1">
         <v>0.96049300000000004</v>
       </c>
+      <c r="AK10">
+        <v>13000</v>
+      </c>
+      <c r="AL10" s="1">
+        <v>33.1413709999999</v>
+      </c>
+      <c r="AM10" s="1">
+        <v>10.900321</v>
+      </c>
+      <c r="AN10" s="1">
+        <v>1.0519270000000001</v>
+      </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>14000</v>
       </c>
@@ -5422,8 +7085,20 @@
       <c r="AB11" s="1">
         <v>1.0596219999999901</v>
       </c>
+      <c r="AK11">
+        <v>14000</v>
+      </c>
+      <c r="AL11" s="1">
+        <v>39.031855999999898</v>
+      </c>
+      <c r="AM11" s="1">
+        <v>12.6462489999999</v>
+      </c>
+      <c r="AN11" s="1">
+        <v>1.2426009999999901</v>
+      </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>15000</v>
       </c>
@@ -5460,8 +7135,20 @@
       <c r="AB12" s="1">
         <v>1.5969629999999999</v>
       </c>
+      <c r="AK12">
+        <v>15000</v>
+      </c>
+      <c r="AL12" s="1">
+        <v>44.075682</v>
+      </c>
+      <c r="AM12" s="1">
+        <v>14.379073999999999</v>
+      </c>
+      <c r="AN12" s="1">
+        <v>1.192161</v>
+      </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>16000</v>
       </c>
@@ -5498,8 +7185,20 @@
       <c r="AB13" s="1">
         <v>1.8700029999999901</v>
       </c>
+      <c r="AK13">
+        <v>16000</v>
+      </c>
+      <c r="AL13" s="1">
+        <v>50.127304000000002</v>
+      </c>
+      <c r="AM13" s="1">
+        <v>16.438334000000001</v>
+      </c>
+      <c r="AN13" s="1">
+        <v>1.5837459999999901</v>
+      </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>17000</v>
       </c>
@@ -5536,8 +7235,20 @@
       <c r="AB14" s="1">
         <v>1.229525</v>
       </c>
+      <c r="AK14">
+        <v>17000</v>
+      </c>
+      <c r="AL14" s="1">
+        <v>56.3362529999999</v>
+      </c>
+      <c r="AM14" s="1">
+        <v>18.819907000000001</v>
+      </c>
+      <c r="AN14" s="1">
+        <v>1.4539679999999999</v>
+      </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>18000</v>
       </c>
@@ -5574,8 +7285,20 @@
       <c r="AB15" s="1">
         <v>1.8255669999999999</v>
       </c>
+      <c r="AK15">
+        <v>18000</v>
+      </c>
+      <c r="AL15" s="1">
+        <v>63.108265999999901</v>
+      </c>
+      <c r="AM15" s="1">
+        <v>20.898319999999899</v>
+      </c>
+      <c r="AN15" s="1">
+        <v>1.653087</v>
+      </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>19000</v>
       </c>
@@ -5612,8 +7335,20 @@
       <c r="AB16" s="1">
         <v>1.4071180000000001</v>
       </c>
+      <c r="AK16">
+        <v>19000</v>
+      </c>
+      <c r="AL16" s="1">
+        <v>70.543727999999902</v>
+      </c>
+      <c r="AM16" s="1">
+        <v>23.544235</v>
+      </c>
+      <c r="AN16" s="1">
+        <v>1.553493</v>
+      </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>20000</v>
       </c>
@@ -5650,8 +7385,20 @@
       <c r="AB17" s="1">
         <v>1.7825629999999999</v>
       </c>
+      <c r="AK17">
+        <v>20000</v>
+      </c>
+      <c r="AL17" s="1">
+        <v>77.884429999999995</v>
+      </c>
+      <c r="AM17" s="1">
+        <v>25.590960999999901</v>
+      </c>
+      <c r="AN17" s="1">
+        <v>1.66315999999999</v>
+      </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>21000</v>
       </c>
@@ -5688,8 +7435,20 @@
       <c r="AB18" s="1">
         <v>1.5264179999999901</v>
       </c>
+      <c r="AK18">
+        <v>21000</v>
+      </c>
+      <c r="AL18" s="1">
+        <v>85.664824999999993</v>
+      </c>
+      <c r="AM18" s="1">
+        <v>28.2793139999999</v>
+      </c>
+      <c r="AN18" s="1">
+        <v>1.79426</v>
+      </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>22000</v>
       </c>
@@ -5726,8 +7485,20 @@
       <c r="AB19" s="1">
         <v>2.1884509999999899</v>
       </c>
+      <c r="AK19">
+        <v>22000</v>
+      </c>
+      <c r="AL19" s="1">
+        <v>94.093359999999905</v>
+      </c>
+      <c r="AM19" s="1">
+        <v>30.854281999999898</v>
+      </c>
+      <c r="AN19" s="1">
+        <v>1.86834199999999</v>
+      </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>23000</v>
       </c>
@@ -5764,8 +7535,20 @@
       <c r="AB20" s="1">
         <v>2.00949</v>
       </c>
+      <c r="AK20">
+        <v>23000</v>
+      </c>
+      <c r="AL20" s="1">
+        <v>102.523113</v>
+      </c>
+      <c r="AM20" s="1">
+        <v>33.615399999999902</v>
+      </c>
+      <c r="AN20" s="1">
+        <v>2.0338910000000001</v>
+      </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>24000</v>
       </c>
@@ -5802,8 +7585,20 @@
       <c r="AB21" s="1">
         <v>2.0369749999999902</v>
       </c>
+      <c r="AK21">
+        <v>24000</v>
+      </c>
+      <c r="AL21" s="1">
+        <v>111.522629999999</v>
+      </c>
+      <c r="AM21" s="1">
+        <v>36.867277999999999</v>
+      </c>
+      <c r="AN21" s="1">
+        <v>2.0497289999999899</v>
+      </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>25000</v>
       </c>
@@ -5840,8 +7635,20 @@
       <c r="AB22" s="1">
         <v>2.2127059999999998</v>
       </c>
+      <c r="AK22">
+        <v>25000</v>
+      </c>
+      <c r="AL22" s="1">
+        <v>123.110223</v>
+      </c>
+      <c r="AM22" s="1">
+        <v>39.903345000000002</v>
+      </c>
+      <c r="AN22" s="1">
+        <v>2.6106019999999899</v>
+      </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>26000</v>
       </c>
@@ -5878,8 +7685,20 @@
       <c r="AB23" s="1">
         <v>3.1870169999999902</v>
       </c>
+      <c r="AK23">
+        <v>26000</v>
+      </c>
+      <c r="AL23" s="1">
+        <v>131.49254999999999</v>
+      </c>
+      <c r="AM23" s="1">
+        <v>42.991053000000001</v>
+      </c>
+      <c r="AN23" s="1">
+        <v>2.7754779999999899</v>
+      </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>27000</v>
       </c>
@@ -5916,8 +7735,20 @@
       <c r="AB24" s="1">
         <v>3.2096290000000001</v>
       </c>
+      <c r="AK24">
+        <v>27000</v>
+      </c>
+      <c r="AL24" s="1">
+        <v>141.08928699999899</v>
+      </c>
+      <c r="AM24" s="1">
+        <v>46.427185999999999</v>
+      </c>
+      <c r="AN24" s="1">
+        <v>2.385783</v>
+      </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>28000</v>
       </c>
@@ -5954,8 +7785,20 @@
       <c r="AB25" s="1">
         <v>2.0717560000000002</v>
       </c>
+      <c r="AK25">
+        <v>28000</v>
+      </c>
+      <c r="AL25" s="1">
+        <v>152.36953800000001</v>
+      </c>
+      <c r="AM25" s="1">
+        <v>51.149076999999998</v>
+      </c>
+      <c r="AN25" s="1">
+        <v>2.3556119999999998</v>
+      </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>29000</v>
       </c>
@@ -5992,8 +7835,20 @@
       <c r="AB26" s="1">
         <v>2.55071099999999</v>
       </c>
+      <c r="AK26">
+        <v>29000</v>
+      </c>
+      <c r="AL26" s="1">
+        <v>163.916898</v>
+      </c>
+      <c r="AM26" s="1">
+        <v>53.728656000000001</v>
+      </c>
+      <c r="AN26" s="1">
+        <v>2.6308769999999999</v>
+      </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>30000</v>
       </c>
@@ -6030,8 +7885,20 @@
       <c r="AB27" s="1">
         <v>2.5583930000000001</v>
       </c>
+      <c r="AK27">
+        <v>30000</v>
+      </c>
+      <c r="AL27" s="1">
+        <v>174.050454</v>
+      </c>
+      <c r="AM27" s="1">
+        <v>59.379022999999897</v>
+      </c>
+      <c r="AN27" s="1">
+        <v>2.3992830000000001</v>
+      </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>31000</v>
       </c>
@@ -6068,8 +7935,20 @@
       <c r="AB28" s="1">
         <v>3.5182220000000002</v>
       </c>
+      <c r="AK28">
+        <v>31000</v>
+      </c>
+      <c r="AL28" s="1">
+        <v>188.60286299999899</v>
+      </c>
+      <c r="AM28" s="1">
+        <v>61.546969999999902</v>
+      </c>
+      <c r="AN28" s="1">
+        <v>2.5101879999999999</v>
+      </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>32000</v>
       </c>
@@ -6106,8 +7985,20 @@
       <c r="AB29" s="1">
         <v>3.7722069999999999</v>
       </c>
+      <c r="AK29">
+        <v>32000</v>
+      </c>
+      <c r="AL29" s="1">
+        <v>200.575853</v>
+      </c>
+      <c r="AM29" s="1">
+        <v>65.790881999999996</v>
+      </c>
+      <c r="AN29" s="1">
+        <v>5.6361590000000001</v>
+      </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>33000</v>
       </c>
@@ -6144,8 +8035,20 @@
       <c r="AB30" s="1">
         <v>4.0346359999999999</v>
       </c>
+      <c r="AK30">
+        <v>33000</v>
+      </c>
+      <c r="AL30" s="1">
+        <v>210.50672599999899</v>
+      </c>
+      <c r="AM30" s="1">
+        <v>70.290911999999906</v>
+      </c>
+      <c r="AN30" s="1">
+        <v>3.6168330000000002</v>
+      </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>34000</v>
       </c>
@@ -6182,8 +8085,20 @@
       <c r="AB31" s="1">
         <v>4.2821759999999998</v>
       </c>
+      <c r="AK31">
+        <v>34000</v>
+      </c>
+      <c r="AL31" s="1">
+        <v>223.73216400000001</v>
+      </c>
+      <c r="AM31" s="1">
+        <v>74.096071999999893</v>
+      </c>
+      <c r="AN31" s="1">
+        <v>4.3688310000000001</v>
+      </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>35000</v>
       </c>
@@ -6220,8 +8135,20 @@
       <c r="AB32" s="1">
         <v>4.926933</v>
       </c>
+      <c r="AK32">
+        <v>35000</v>
+      </c>
+      <c r="AL32" s="1">
+        <v>237.09723399999999</v>
+      </c>
+      <c r="AM32" s="1">
+        <v>78.308682999999903</v>
+      </c>
+      <c r="AN32" s="1">
+        <v>3.4384079999999999</v>
+      </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>

</xml_diff>